<commit_message>
perbaiki dokumen pembukaan penawaran dan evaluasi satu sampul (kecuali lampiran)
</commit_message>
<xml_diff>
--- a/templates/10.a-Lam BA PEMBUKAAN 1 Sampul.xlsx
+++ b/templates/10.a-Lam BA PEMBUKAAN 1 Sampul.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="255" windowWidth="9780" windowHeight="5835" tabRatio="602"/>
@@ -850,241 +850,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Nomor :  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#nomor#</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, Tanggal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tgllengkap#</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Pada hari  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#hari#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tanggal  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tanggal#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Bulan #bulan# Tahun </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tahun#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tgllengkap#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) Jam </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#jam#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Wib, bertempat di </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tempat#,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#panitia#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (Persero) Kantor Pusat yang dibentuk sesuai Surat Keputusan Direksi Nomor : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#nosk#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tanggal  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tglsk#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> telah melakukan Pembukaan Penawaran Harga Pekerjaan </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#namapengadaan#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> yang dihadiri oleh </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#panitia#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> dan Penyedia Barang/Jasa sebagai berikut :</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">PEKERJAAN PENGADAAN  </t>
     </r>
     <r>
@@ -1224,18 +989,24 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>Pada hari  #hari# tanggal  #tanggal# Bulan #bulan# Tahun #tahun# (#tgllengkap#) Pukul #jam# Wib, bertempat di #tempat#, #panitia# (Persero) Kantor Pusat #kalimatpanitia# telah melakukan Pembukaan Penawaran Harga Pekerjaan #namapengadaan# yang dihadiri oleh #panitia# dan Penyedia Barang/Jasa sebagai berikut :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomor :  #nomor#, Tanggal #tgllengkap# </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$Rp-421]#,##0.00;[Red][$Rp-421]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$Rp-421]#,##0.00;[Red][$Rp-421]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="40">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1243,6 +1014,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2695,10 +2467,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="309">
+  <cellXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3050,24 +2822,24 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3237,7 +3009,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3390,13 +3162,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3448,6 +3220,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3508,7 +3283,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3543,7 +3318,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3566,14 +3341,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3626,7 +3401,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3912,7 +3687,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3947,7 +3721,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4123,14 +3896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48:F49"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
@@ -4145,19 +3918,19 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10">
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10">
       <c r="C3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="18">
       <c r="C4" s="71"/>
       <c r="D4" s="71"/>
       <c r="E4" s="71"/>
@@ -4166,7 +3939,7 @@
       <c r="H4" s="71"/>
       <c r="I4" s="71"/>
     </row>
-    <row r="5" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="18" customHeight="1">
       <c r="B5" s="237" t="s">
         <v>9</v>
       </c>
@@ -4179,20 +3952,20 @@
       <c r="I5" s="30"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="237" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
-      <c r="E6" s="237"/>
-      <c r="F6" s="237"/>
-      <c r="G6" s="237"/>
-      <c r="H6" s="237"/>
+    <row r="6" spans="2:10" ht="18" customHeight="1">
+      <c r="B6" s="309" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="309"/>
+      <c r="D6" s="309"/>
+      <c r="E6" s="309"/>
+      <c r="F6" s="309"/>
+      <c r="G6" s="309"/>
+      <c r="H6" s="309"/>
       <c r="I6" s="30"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="18" customHeight="1">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4203,10 +3976,10 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="96" customHeight="1">
       <c r="B8" s="5"/>
       <c r="C8" s="238" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D8" s="238"/>
       <c r="E8" s="238"/>
@@ -4216,7 +3989,7 @@
       <c r="I8" s="31"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="14.1" customHeight="1">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4227,7 +4000,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" ht="12.75" customHeight="1">
       <c r="B10" s="40"/>
       <c r="C10" s="41"/>
       <c r="D10" s="42"/>
@@ -4240,7 +4013,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="12.75" customHeight="1">
       <c r="B11" s="43"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
@@ -4251,7 +4024,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1">
       <c r="B12" s="45" t="s">
         <v>0</v>
       </c>
@@ -4272,7 +4045,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="15.75">
       <c r="B13" s="45" t="s">
         <v>1</v>
       </c>
@@ -4285,7 +4058,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="15">
       <c r="B14" s="45"/>
       <c r="C14" s="228" t="s">
         <v>32</v>
@@ -4298,7 +4071,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="12.75" customHeight="1">
       <c r="B15" s="45"/>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
@@ -4314,7 +4087,7 @@
       </c>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="12.75" customHeight="1">
       <c r="B16" s="45"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
@@ -4324,7 +4097,7 @@
       <c r="H16" s="231"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" ht="12.75" customHeight="1">
       <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
@@ -4341,7 +4114,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" ht="15.95" customHeight="1">
       <c r="B18" s="47"/>
       <c r="C18" s="16"/>
       <c r="D18" s="15"/>
@@ -4351,7 +4124,7 @@
       <c r="H18" s="47"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15.95" customHeight="1">
       <c r="B19" s="44" t="s">
         <v>4</v>
       </c>
@@ -4366,7 +4139,7 @@
       <c r="I19" s="17"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="15.95" customHeight="1">
       <c r="B20" s="56">
         <v>1</v>
       </c>
@@ -4381,7 +4154,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" ht="15.95" customHeight="1">
       <c r="B21" s="56"/>
       <c r="C21" s="54" t="s">
         <v>25</v>
@@ -4398,7 +4171,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" ht="15.95" customHeight="1">
       <c r="B22" s="56"/>
       <c r="C22" s="54" t="s">
         <v>28</v>
@@ -4415,7 +4188,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" ht="15.95" customHeight="1">
       <c r="B23" s="56">
         <v>2</v>
       </c>
@@ -4434,7 +4207,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" ht="15.95" customHeight="1">
       <c r="B24" s="56">
         <v>3</v>
       </c>
@@ -4453,7 +4226,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10">
       <c r="B25" s="56">
         <v>4</v>
       </c>
@@ -4472,7 +4245,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10">
       <c r="B26" s="56">
         <v>5</v>
       </c>
@@ -4491,7 +4264,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10">
       <c r="B27" s="56">
         <v>6</v>
       </c>
@@ -4510,7 +4283,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="13.5" thickBot="1">
       <c r="B28" s="43"/>
       <c r="C28" s="7"/>
       <c r="D28" s="6"/>
@@ -4521,7 +4294,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="2:10" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="15.95" customHeight="1" thickBot="1">
       <c r="B29" s="48"/>
       <c r="C29" s="50" t="s">
         <v>3</v>
@@ -4540,7 +4313,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="15.75">
       <c r="B30" s="44" t="s">
         <v>5</v>
       </c>
@@ -4555,7 +4328,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" ht="15">
       <c r="B31" s="56"/>
       <c r="C31" s="61"/>
       <c r="D31" s="55"/>
@@ -4566,7 +4339,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" ht="15">
       <c r="B32" s="56">
         <v>1</v>
       </c>
@@ -4587,7 +4360,7 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="2:36" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:36" ht="15">
       <c r="B33" s="56">
         <v>2</v>
       </c>
@@ -4608,7 +4381,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="2:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:36" ht="18" customHeight="1">
       <c r="B34" s="56">
         <v>3</v>
       </c>
@@ -4629,7 +4402,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="2:36" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:36" ht="18" customHeight="1" thickBot="1">
       <c r="B35" s="43"/>
       <c r="C35" s="53"/>
       <c r="D35" s="6"/>
@@ -4639,7 +4412,7 @@
       <c r="H35" s="45"/>
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="2:36" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:36" ht="13.5" thickBot="1">
       <c r="B36" s="48"/>
       <c r="C36" s="50" t="s">
         <v>21</v>
@@ -4683,7 +4456,7 @@
       <c r="AI36" s="20"/>
       <c r="AJ36" s="20"/>
     </row>
-    <row r="37" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:36">
       <c r="B37" s="83"/>
       <c r="C37" s="83"/>
       <c r="D37" s="83"/>
@@ -4719,7 +4492,7 @@
       <c r="AI37" s="20"/>
       <c r="AJ37" s="20"/>
     </row>
-    <row r="38" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:36">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -4755,7 +4528,7 @@
       <c r="AI38" s="20"/>
       <c r="AJ38" s="20"/>
     </row>
-    <row r="39" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:36">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -4791,7 +4564,7 @@
       <c r="AI39" s="20"/>
       <c r="AJ39" s="20"/>
     </row>
-    <row r="40" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:36">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -4827,7 +4600,7 @@
       <c r="AI40" s="20"/>
       <c r="AJ40" s="20"/>
     </row>
-    <row r="41" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:36">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -4863,7 +4636,7 @@
       <c r="AI41" s="20"/>
       <c r="AJ41" s="20"/>
     </row>
-    <row r="42" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:36">
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
       <c r="D42" s="52"/>
@@ -4899,7 +4672,7 @@
       <c r="AI42" s="20"/>
       <c r="AJ42" s="20"/>
     </row>
-    <row r="43" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:36" ht="12.75" customHeight="1">
       <c r="B43" s="40"/>
       <c r="C43" s="41"/>
       <c r="D43" s="42"/>
@@ -4912,7 +4685,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:36" ht="12.75" customHeight="1">
       <c r="B44" s="43"/>
       <c r="C44" s="7"/>
       <c r="D44" s="6"/>
@@ -4923,7 +4696,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="9"/>
     </row>
-    <row r="45" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:36" ht="15.75" customHeight="1">
       <c r="B45" s="45" t="s">
         <v>0</v>
       </c>
@@ -4944,7 +4717,7 @@
       <c r="I45" s="10"/>
       <c r="J45" s="11"/>
     </row>
-    <row r="46" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:36" ht="15.75">
       <c r="B46" s="45" t="s">
         <v>1</v>
       </c>
@@ -4957,7 +4730,7 @@
       <c r="I46" s="10"/>
       <c r="J46" s="11"/>
     </row>
-    <row r="47" spans="2:36" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:36" ht="15">
       <c r="B47" s="45"/>
       <c r="C47" s="228" t="s">
         <v>32</v>
@@ -4970,7 +4743,7 @@
       <c r="I47" s="12"/>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:36" ht="12.75" customHeight="1">
       <c r="B48" s="45"/>
       <c r="C48" s="7"/>
       <c r="D48" s="6"/>
@@ -4986,7 +4759,7 @@
       </c>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="2:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:36" ht="12.75" customHeight="1">
       <c r="B49" s="45"/>
       <c r="C49" s="7"/>
       <c r="D49" s="6"/>
@@ -4996,7 +4769,7 @@
       <c r="H49" s="231"/>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="2:36" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:36" ht="12.75" customHeight="1" thickBot="1">
       <c r="B50" s="88"/>
       <c r="C50" s="89"/>
       <c r="D50" s="90"/>
@@ -5013,7 +4786,7 @@
       <c r="I50" s="14"/>
       <c r="J50" s="15"/>
     </row>
-    <row r="51" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:36">
       <c r="B51" s="43"/>
       <c r="C51" s="7"/>
       <c r="D51" s="6"/>
@@ -5049,7 +4822,7 @@
       <c r="AI51" s="20"/>
       <c r="AJ51" s="20"/>
     </row>
-    <row r="52" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:36">
       <c r="B52" s="44" t="s">
         <v>6</v>
       </c>
@@ -5095,7 +4868,7 @@
       <c r="AI52" s="20"/>
       <c r="AJ52" s="20"/>
     </row>
-    <row r="53" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:36">
       <c r="B53" s="56"/>
       <c r="C53" s="54" t="s">
         <v>10</v>
@@ -5133,7 +4906,7 @@
       <c r="AI53" s="20"/>
       <c r="AJ53" s="20"/>
     </row>
-    <row r="54" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:36">
       <c r="B54" s="56"/>
       <c r="C54" s="54" t="s">
         <v>8</v>
@@ -5171,7 +4944,7 @@
       <c r="AI54" s="20"/>
       <c r="AJ54" s="20"/>
     </row>
-    <row r="55" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:36">
       <c r="B55" s="56"/>
       <c r="C55" s="54" t="s">
         <v>39</v>
@@ -5209,7 +4982,7 @@
       <c r="AI55" s="20"/>
       <c r="AJ55" s="20"/>
     </row>
-    <row r="56" spans="2:36" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:36" ht="13.5" thickBot="1">
       <c r="B56" s="49"/>
       <c r="C56" s="51" t="s">
         <v>53</v>
@@ -5247,7 +5020,7 @@
       <c r="AI56" s="20"/>
       <c r="AJ56" s="20"/>
     </row>
-    <row r="57" spans="2:36" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:36" ht="13.5" thickBot="1">
       <c r="B57" s="48"/>
       <c r="C57" s="50" t="s">
         <v>21</v>
@@ -5291,7 +5064,7 @@
       <c r="AI57" s="20"/>
       <c r="AJ57" s="20"/>
     </row>
-    <row r="58" spans="2:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:36" ht="20.100000000000001" customHeight="1">
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -5301,7 +5074,7 @@
       <c r="H58" s="10"/>
       <c r="J58" s="6"/>
     </row>
-    <row r="59" spans="2:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:36" ht="20.100000000000001" customHeight="1">
       <c r="B59" s="74" t="s">
         <v>11</v>
       </c>
@@ -5309,13 +5082,13 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="2:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:36" ht="20.100000000000001" customHeight="1">
       <c r="B60" s="234" t="s">
         <v>13</v>
       </c>
@@ -5323,13 +5096,13 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="2:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:36" ht="20.100000000000001" customHeight="1">
       <c r="B61" s="234" t="s">
         <v>12</v>
       </c>
@@ -5343,7 +5116,7 @@
       <c r="H61" s="6"/>
       <c r="J61" s="6"/>
     </row>
-    <row r="62" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:36">
       <c r="B62" s="51" t="s">
         <v>16</v>
       </c>
@@ -5354,7 +5127,7 @@
       <c r="H62" s="6"/>
       <c r="J62" s="6"/>
     </row>
-    <row r="63" spans="2:36" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:36" ht="15">
       <c r="B63" s="6"/>
       <c r="C63" s="66"/>
       <c r="D63" s="14"/>
@@ -5368,7 +5141,7 @@
       <c r="I63" s="14"/>
       <c r="J63" s="6"/>
     </row>
-    <row r="64" spans="2:36" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:36" ht="15">
       <c r="B64" s="236" t="s">
         <v>43</v>
       </c>
@@ -5381,7 +5154,7 @@
       <c r="G64" s="24"/>
       <c r="J64" s="6"/>
     </row>
-    <row r="65" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:10" ht="15">
       <c r="B65" s="6"/>
       <c r="C65" s="66"/>
       <c r="D65" s="14"/>
@@ -5391,7 +5164,7 @@
       <c r="I65" s="17"/>
       <c r="J65" s="6"/>
     </row>
-    <row r="66" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:10" ht="15">
       <c r="B66" s="233"/>
       <c r="C66" s="233"/>
       <c r="D66" s="14"/>
@@ -5405,7 +5178,7 @@
       <c r="I66" s="17"/>
       <c r="J66" s="6"/>
     </row>
-    <row r="67" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:10" ht="15">
       <c r="B67" s="232"/>
       <c r="C67" s="232"/>
       <c r="D67" s="14"/>
@@ -5417,7 +5190,7 @@
       <c r="I67" s="17"/>
       <c r="J67" s="6"/>
     </row>
-    <row r="68" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:10" ht="15">
       <c r="B68" s="232"/>
       <c r="C68" s="232"/>
       <c r="D68" s="14"/>
@@ -5427,7 +5200,7 @@
       <c r="I68" s="17"/>
       <c r="J68" s="6"/>
     </row>
-    <row r="69" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10" ht="15">
       <c r="B69" s="6"/>
       <c r="C69" s="66"/>
       <c r="D69" s="14"/>
@@ -5441,7 +5214,7 @@
       <c r="I69" s="17"/>
       <c r="J69" s="6"/>
     </row>
-    <row r="70" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:10" ht="15">
       <c r="B70" s="233" t="s">
         <v>45</v>
       </c>
@@ -5455,7 +5228,7 @@
       <c r="I70" s="17"/>
       <c r="J70" s="6"/>
     </row>
-    <row r="71" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:10" ht="15">
       <c r="B71" s="6"/>
       <c r="C71" s="66"/>
       <c r="D71" s="14"/>
@@ -5465,7 +5238,7 @@
       <c r="I71" s="17"/>
       <c r="J71" s="6"/>
     </row>
-    <row r="72" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:10" ht="15">
       <c r="B72" s="233"/>
       <c r="C72" s="233"/>
       <c r="D72" s="14"/>
@@ -5475,7 +5248,7 @@
       <c r="I72" s="17"/>
       <c r="J72" s="6"/>
     </row>
-    <row r="73" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:10" ht="15">
       <c r="B73" s="232"/>
       <c r="C73" s="232"/>
       <c r="D73" s="14"/>
@@ -5485,7 +5258,7 @@
       <c r="I73" s="17"/>
       <c r="J73" s="6"/>
     </row>
-    <row r="74" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:10" ht="15">
       <c r="B74" s="232"/>
       <c r="C74" s="232"/>
       <c r="D74" s="14"/>
@@ -5495,7 +5268,7 @@
       <c r="I74" s="17"/>
       <c r="J74" s="6"/>
     </row>
-    <row r="75" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:10" ht="15">
       <c r="B75" s="6"/>
       <c r="C75" s="66"/>
       <c r="D75" s="14"/>
@@ -5505,7 +5278,7 @@
       <c r="I75" s="14"/>
       <c r="J75" s="6"/>
     </row>
-    <row r="76" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10" ht="15">
       <c r="B76" s="233" t="s">
         <v>45</v>
       </c>
@@ -5517,7 +5290,7 @@
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
     </row>
-    <row r="77" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:10" ht="15">
       <c r="B77" s="6"/>
       <c r="C77" s="35"/>
       <c r="D77" s="14"/>
@@ -5527,7 +5300,7 @@
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
     </row>
-    <row r="78" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:10" ht="15">
       <c r="B78" s="233"/>
       <c r="C78" s="233"/>
       <c r="D78" s="14"/>
@@ -5537,7 +5310,7 @@
       <c r="I78" s="14"/>
       <c r="J78" s="6"/>
     </row>
-    <row r="79" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:10" ht="15">
       <c r="B79" s="232"/>
       <c r="C79" s="232"/>
       <c r="D79" s="14"/>
@@ -5547,7 +5320,7 @@
       <c r="I79" s="6"/>
       <c r="J79" s="6"/>
     </row>
-    <row r="80" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:10" ht="15">
       <c r="B80" s="232"/>
       <c r="C80" s="232"/>
       <c r="D80" s="14"/>
@@ -5557,7 +5330,7 @@
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
     </row>
-    <row r="81" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:10" ht="15">
       <c r="B81" s="6"/>
       <c r="C81" s="66"/>
       <c r="D81" s="26"/>
@@ -5567,7 +5340,7 @@
       <c r="I81" s="14"/>
       <c r="J81" s="6"/>
     </row>
-    <row r="82" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:10" ht="15">
       <c r="B82" s="233" t="s">
         <v>45</v>
       </c>
@@ -5579,7 +5352,7 @@
       <c r="I82" s="6"/>
       <c r="J82" s="6"/>
     </row>
-    <row r="83" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:10" ht="15">
       <c r="C83" s="35"/>
       <c r="D83" s="27"/>
       <c r="E83" s="5"/>
@@ -5588,7 +5361,7 @@
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
     </row>
-    <row r="84" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:10" ht="15">
       <c r="C84" s="36"/>
       <c r="D84" s="26"/>
       <c r="E84" s="37"/>
@@ -5597,7 +5370,7 @@
       <c r="I84" s="14"/>
       <c r="J84" s="6"/>
     </row>
-    <row r="85" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:10" ht="15">
       <c r="C85" s="33"/>
       <c r="D85" s="27"/>
       <c r="E85" s="5"/>
@@ -5606,7 +5379,7 @@
       <c r="I85" s="6"/>
       <c r="J85" s="6"/>
     </row>
-    <row r="86" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:10" ht="15">
       <c r="C86" s="36"/>
       <c r="D86" s="26"/>
       <c r="E86" s="5"/>
@@ -5615,7 +5388,7 @@
       <c r="I86" s="6"/>
       <c r="J86" s="6"/>
     </row>
-    <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:10" ht="15">
       <c r="C87" s="36"/>
       <c r="D87" s="26"/>
       <c r="E87" s="37"/>
@@ -5624,7 +5397,7 @@
       <c r="I87" s="14"/>
       <c r="J87" s="6"/>
     </row>
-    <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:10" ht="15">
       <c r="C88" s="33"/>
       <c r="D88" s="26"/>
       <c r="E88" s="5"/>
@@ -5633,7 +5406,7 @@
       <c r="H88" s="6"/>
       <c r="J88" s="6"/>
     </row>
-    <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:10" ht="15">
       <c r="C89" s="36"/>
       <c r="D89" s="26"/>
       <c r="E89" s="25"/>
@@ -5642,14 +5415,14 @@
       <c r="H89" s="6"/>
       <c r="J89" s="6"/>
     </row>
-    <row r="90" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:10" ht="15">
       <c r="C90" s="32"/>
       <c r="D90" s="27"/>
       <c r="F90" s="26"/>
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
     </row>
-    <row r="91" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:10" ht="15">
       <c r="B91" s="6"/>
       <c r="C91" s="34"/>
       <c r="D91" s="26"/>
@@ -5657,7 +5430,7 @@
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
     </row>
-    <row r="92" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:10" ht="15">
       <c r="B92" s="6"/>
       <c r="C92" s="34"/>
       <c r="D92" s="26"/>
@@ -5665,7 +5438,7 @@
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
     </row>
-    <row r="93" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:10" ht="15">
       <c r="B93" s="6"/>
       <c r="C93" s="32"/>
       <c r="D93" s="27"/>
@@ -5673,7 +5446,7 @@
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
     </row>
-    <row r="94" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:10" ht="15">
       <c r="B94" s="6"/>
       <c r="C94" s="34"/>
       <c r="D94" s="26"/>
@@ -5681,7 +5454,7 @@
       <c r="G94" s="6"/>
       <c r="H94" s="6"/>
     </row>
-    <row r="95" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:10" ht="15">
       <c r="B95" s="6"/>
       <c r="C95" s="32"/>
       <c r="D95" s="27"/>
@@ -5689,7 +5462,7 @@
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
     </row>
-    <row r="96" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:10" ht="15">
       <c r="B96" s="6"/>
       <c r="C96" s="34"/>
       <c r="D96" s="21"/>
@@ -5697,7 +5470,7 @@
       <c r="G96" s="6"/>
       <c r="H96" s="6"/>
     </row>
-    <row r="97" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:8" ht="15">
       <c r="B97" s="6"/>
       <c r="C97" s="32"/>
       <c r="D97" s="27"/>
@@ -5705,7 +5478,7 @@
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:8">
       <c r="B98" s="6"/>
       <c r="C98" s="26"/>
       <c r="D98" s="26"/>
@@ -5714,7 +5487,7 @@
       <c r="G98" s="6"/>
       <c r="H98" s="6"/>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:8">
       <c r="B99" s="6"/>
       <c r="C99" s="14"/>
       <c r="D99" s="27"/>
@@ -5723,37 +5496,37 @@
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:8">
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:8">
       <c r="B101" s="6"/>
       <c r="C101" s="68"/>
       <c r="D101" s="69"/>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:8">
       <c r="B102" s="6"/>
       <c r="C102" s="227"/>
       <c r="D102" s="227"/>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:8">
       <c r="B103" s="6"/>
       <c r="C103" s="227"/>
       <c r="D103" s="227"/>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:8">
       <c r="B104" s="6"/>
       <c r="C104" s="23"/>
       <c r="D104" s="23"/>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:8">
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:8">
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
@@ -5811,32 +5584,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="13.5">
       <c r="J2" s="199" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="13.5">
       <c r="J3" s="199" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16.5">
       <c r="A4" s="200"/>
     </row>
-    <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="16.5">
       <c r="A5" s="251" t="s">
         <v>98</v>
       </c>
@@ -5851,9 +5624,9 @@
       <c r="J5" s="251"/>
       <c r="K5" s="251"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="17.25" thickBot="1">
       <c r="A6" s="252" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B6" s="252"/>
       <c r="C6" s="252"/>
@@ -5866,7 +5639,7 @@
       <c r="J6" s="252"/>
       <c r="K6" s="252"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A7" s="201" t="s">
         <v>66</v>
       </c>
@@ -5890,7 +5663,7 @@
       </c>
       <c r="L7" s="203"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="204"/>
       <c r="B8" s="280" t="s">
         <v>103</v>
@@ -5910,7 +5683,7 @@
       <c r="K8" s="205"/>
       <c r="L8" s="203"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="204" t="s">
         <v>4</v>
       </c>
@@ -5932,7 +5705,7 @@
       <c r="K9" s="205"/>
       <c r="L9" s="203"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1">
       <c r="A10" s="206">
         <v>1</v>
       </c>
@@ -5954,7 +5727,7 @@
       <c r="K10" s="205"/>
       <c r="L10" s="203"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1">
       <c r="A11" s="206"/>
       <c r="B11" s="268" t="s">
         <v>108</v>
@@ -5974,7 +5747,7 @@
       <c r="K11" s="205"/>
       <c r="L11" s="203"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1">
       <c r="A12" s="206"/>
       <c r="B12" s="268" t="s">
         <v>109</v>
@@ -5994,7 +5767,7 @@
       <c r="K12" s="205"/>
       <c r="L12" s="203"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="A13" s="206"/>
       <c r="B13" s="268" t="s">
         <v>110</v>
@@ -6014,7 +5787,7 @@
       <c r="K13" s="205"/>
       <c r="L13" s="203"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="A14" s="206"/>
       <c r="B14" s="268" t="s">
         <v>111</v>
@@ -6034,7 +5807,7 @@
       <c r="K14" s="205"/>
       <c r="L14" s="203"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.75" thickBot="1">
       <c r="A15" s="206"/>
       <c r="B15" s="268" t="s">
         <v>112</v>
@@ -6054,7 +5827,7 @@
       <c r="K15" s="205"/>
       <c r="L15" s="203"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.75" thickBot="1">
       <c r="A16" s="206">
         <v>2</v>
       </c>
@@ -6076,7 +5849,7 @@
       <c r="K16" s="205"/>
       <c r="L16" s="203"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1">
       <c r="A17" s="207">
         <v>3</v>
       </c>
@@ -6098,7 +5871,7 @@
       <c r="K17" s="208"/>
       <c r="L17" s="203"/>
     </row>
-    <row r="18" spans="1:12" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="25.5" customHeight="1" thickBot="1">
       <c r="A18" s="206">
         <v>4</v>
       </c>
@@ -6120,7 +5893,7 @@
       <c r="K18" s="205"/>
       <c r="L18" s="203"/>
     </row>
-    <row r="19" spans="1:12" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="206">
         <v>5</v>
       </c>
@@ -6142,7 +5915,7 @@
       <c r="K19" s="205"/>
       <c r="L19" s="203"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1">
       <c r="A20" s="206">
         <v>6</v>
       </c>
@@ -6164,7 +5937,7 @@
       <c r="K20" s="205"/>
       <c r="L20" s="203"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1">
       <c r="A21" s="204" t="s">
         <v>5</v>
       </c>
@@ -6186,7 +5959,7 @@
       <c r="K21" s="205"/>
       <c r="L21" s="203"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
       <c r="A22" s="206">
         <v>1</v>
       </c>
@@ -6208,7 +5981,7 @@
       <c r="K22" s="205"/>
       <c r="L22" s="203"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1">
       <c r="A23" s="206">
         <v>2</v>
       </c>
@@ -6230,7 +6003,7 @@
       <c r="K23" s="205"/>
       <c r="L23" s="203"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1">
       <c r="A24" s="206">
         <v>3</v>
       </c>
@@ -6252,7 +6025,7 @@
       <c r="K24" s="205"/>
       <c r="L24" s="203"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
       <c r="A25" s="206">
         <v>4</v>
       </c>
@@ -6274,7 +6047,7 @@
       <c r="K25" s="205"/>
       <c r="L25" s="203"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1">
       <c r="A26" s="206">
         <v>5</v>
       </c>
@@ -6296,7 +6069,7 @@
       <c r="K26" s="205"/>
       <c r="L26" s="203"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15.75" thickBot="1">
       <c r="A27" s="204" t="s">
         <v>6</v>
       </c>
@@ -6318,7 +6091,7 @@
       <c r="K27" s="205"/>
       <c r="L27" s="203"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
       <c r="A28" s="204"/>
       <c r="B28" s="268" t="s">
         <v>125</v>
@@ -6338,7 +6111,7 @@
       <c r="K28" s="205"/>
       <c r="L28" s="203"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15.75" thickBot="1">
       <c r="A29" s="214"/>
       <c r="B29" s="215"/>
       <c r="C29" s="216"/>
@@ -6352,7 +6125,7 @@
       <c r="K29" s="221"/>
       <c r="L29" s="203"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1">
       <c r="A30" s="209"/>
       <c r="B30" s="254" t="s">
         <v>128</v>
@@ -6372,7 +6145,7 @@
       <c r="K30" s="210"/>
       <c r="L30" s="203"/>
     </row>
-    <row r="31" spans="1:12" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="14.25" thickTop="1">
       <c r="A31" s="260" t="s">
         <v>128</v>
       </c>
@@ -6381,7 +6154,7 @@
       <c r="E31" s="248"/>
       <c r="F31" s="248"/>
       <c r="G31" s="249" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H31" s="249"/>
       <c r="I31" s="249"/>
@@ -6389,7 +6162,7 @@
       <c r="K31" s="249"/>
       <c r="L31" s="249"/>
     </row>
-    <row r="32" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="27" customHeight="1">
       <c r="A32" s="261" t="s">
         <v>130</v>
       </c>
@@ -6406,7 +6179,7 @@
       <c r="K32" s="249"/>
       <c r="L32" s="249"/>
     </row>
-    <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="13.5" customHeight="1">
       <c r="A33" s="261" t="s">
         <v>131</v>
       </c>
@@ -6424,7 +6197,7 @@
       <c r="K33" s="246"/>
       <c r="L33" s="246"/>
     </row>
-    <row r="34" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="24" customHeight="1">
       <c r="A34" s="261" t="s">
         <v>139</v>
       </c>
@@ -6438,7 +6211,7 @@
       <c r="K34" s="246"/>
       <c r="L34" s="246"/>
     </row>
-    <row r="35" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="27" customHeight="1">
       <c r="A35" s="250"/>
       <c r="B35" s="250"/>
       <c r="D35" s="253" t="s">
@@ -6453,7 +6226,7 @@
       <c r="K35" s="246"/>
       <c r="L35" s="246"/>
     </row>
-    <row r="36" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A36" s="250"/>
       <c r="B36" s="250"/>
       <c r="D36" s="222"/>
@@ -6465,7 +6238,7 @@
       <c r="K36" s="246"/>
       <c r="L36" s="246"/>
     </row>
-    <row r="37" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A37" s="250"/>
       <c r="B37" s="250"/>
       <c r="D37" s="212"/>
@@ -6477,7 +6250,7 @@
       <c r="K37" s="246"/>
       <c r="L37" s="246"/>
     </row>
-    <row r="38" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="13.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A38" s="250"/>
       <c r="B38" s="250"/>
       <c r="D38" s="211"/>
@@ -6489,7 +6262,7 @@
       <c r="K38" s="246"/>
       <c r="L38" s="246"/>
     </row>
-    <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="14.25" customHeight="1">
       <c r="B39" s="211"/>
       <c r="D39" s="212" t="s">
         <v>133</v>
@@ -6506,7 +6279,7 @@
       <c r="K39" s="246"/>
       <c r="L39" s="246"/>
     </row>
-    <row r="40" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="13.5" customHeight="1">
       <c r="B40" s="211"/>
       <c r="C40">
         <v>1</v>
@@ -6524,30 +6297,30 @@
       <c r="K40" s="246"/>
       <c r="L40" s="246"/>
     </row>
-    <row r="41" spans="1:12" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="13.5">
       <c r="D41" s="212"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="D42" s="211"/>
     </row>
-    <row r="43" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="36.75" customHeight="1">
       <c r="D43" s="245" t="s">
         <v>134</v>
       </c>
       <c r="E43" s="245"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="C44">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="13.5">
       <c r="D47" s="245" t="s">
         <v>141</v>
       </c>
       <c r="E47" s="245"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" s="211"/>
     </row>
   </sheetData>
@@ -6648,14 +6421,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B71" sqref="B71:C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="8.140625" customWidth="1"/>
     <col min="3" max="3" width="121.85546875" customWidth="1"/>
@@ -6667,7 +6440,7 @@
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="196"/>
       <c r="B1" s="197"/>
       <c r="C1" s="198"/>
@@ -6679,7 +6452,7 @@
       <c r="G1" s="103"/>
       <c r="H1" s="103"/>
     </row>
-    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="291" t="s">
         <v>64</v>
       </c>
@@ -6692,9 +6465,9 @@
       <c r="H2" s="291"/>
       <c r="I2" s="291"/>
     </row>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="237" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" s="237"/>
       <c r="C3" s="237"/>
@@ -6705,7 +6478,7 @@
       <c r="H3" s="237"/>
       <c r="I3" s="237"/>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="237" t="s">
         <v>65</v>
       </c>
@@ -6718,7 +6491,7 @@
       <c r="H4" s="237"/>
       <c r="I4" s="237"/>
     </row>
-    <row r="5" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.5" thickBot="1">
       <c r="A5" s="104"/>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -6728,7 +6501,7 @@
       <c r="G5" s="104"/>
       <c r="H5" s="104"/>
     </row>
-    <row r="6" spans="1:9" s="106" customFormat="1" ht="21" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="106" customFormat="1" ht="21" thickTop="1">
       <c r="A6" s="292" t="s">
         <v>66</v>
       </c>
@@ -6745,7 +6518,7 @@
       <c r="H6" s="297"/>
       <c r="I6" s="298"/>
     </row>
-    <row r="7" spans="1:9" s="106" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="106" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
       <c r="A7" s="293"/>
       <c r="B7" s="107"/>
       <c r="C7" s="295"/>
@@ -6764,7 +6537,7 @@
       <c r="H7" s="109"/>
       <c r="I7" s="110"/>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
       <c r="A8" s="111">
         <v>1</v>
       </c>
@@ -6791,7 +6564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="36.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="118" t="s">
         <v>63</v>
       </c>
@@ -6806,7 +6579,7 @@
       <c r="H9" s="123"/>
       <c r="I9" s="124"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" thickTop="1">
       <c r="A10" s="125"/>
       <c r="B10" s="126"/>
       <c r="C10" s="127"/>
@@ -6817,7 +6590,7 @@
       <c r="H10" s="130"/>
       <c r="I10" s="131"/>
     </row>
-    <row r="11" spans="1:9" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="20.25">
       <c r="A11" s="299"/>
       <c r="B11" s="300"/>
       <c r="C11" s="301"/>
@@ -6840,7 +6613,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" hidden="1">
       <c r="A12" s="135"/>
       <c r="B12" s="136"/>
       <c r="C12" s="137"/>
@@ -6851,7 +6624,7 @@
       <c r="H12" s="139"/>
       <c r="I12" s="140"/>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="141">
         <v>1</v>
       </c>
@@ -6868,7 +6641,7 @@
       <c r="H13" s="144"/>
       <c r="I13" s="145"/>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="141">
         <v>2</v>
       </c>
@@ -6885,7 +6658,7 @@
       <c r="H14" s="144"/>
       <c r="I14" s="145"/>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="141">
         <v>3</v>
       </c>
@@ -6902,7 +6675,7 @@
       <c r="H15" s="144"/>
       <c r="I15" s="145"/>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="141">
         <v>4</v>
       </c>
@@ -6919,7 +6692,7 @@
       <c r="H16" s="144"/>
       <c r="I16" s="145"/>
     </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="146">
         <v>5</v>
       </c>
@@ -6936,7 +6709,7 @@
       <c r="H17" s="144"/>
       <c r="I17" s="145"/>
     </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="141">
         <v>6</v>
       </c>
@@ -6953,7 +6726,7 @@
       <c r="H18" s="144"/>
       <c r="I18" s="145"/>
     </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="141">
         <v>7</v>
       </c>
@@ -6970,7 +6743,7 @@
       <c r="H19" s="144"/>
       <c r="I19" s="145"/>
     </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="141">
         <v>8</v>
       </c>
@@ -6985,7 +6758,7 @@
       <c r="H20" s="144"/>
       <c r="I20" s="145"/>
     </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="141">
         <v>9</v>
       </c>
@@ -7000,7 +6773,7 @@
       <c r="H21" s="144"/>
       <c r="I21" s="145"/>
     </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="141">
         <v>10</v>
       </c>
@@ -7015,7 +6788,7 @@
       <c r="H22" s="144"/>
       <c r="I22" s="145"/>
     </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="141">
         <v>11</v>
       </c>
@@ -7030,7 +6803,7 @@
       <c r="H23" s="144"/>
       <c r="I23" s="145"/>
     </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="141">
         <v>12</v>
       </c>
@@ -7045,7 +6818,7 @@
       <c r="H24" s="144"/>
       <c r="I24" s="145"/>
     </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="141">
         <v>13</v>
       </c>
@@ -7060,7 +6833,7 @@
       <c r="H25" s="144"/>
       <c r="I25" s="145"/>
     </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="141">
         <v>14</v>
       </c>
@@ -7075,7 +6848,7 @@
       <c r="H26" s="144"/>
       <c r="I26" s="145"/>
     </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="141">
         <v>15</v>
       </c>
@@ -7090,7 +6863,7 @@
       <c r="H27" s="144"/>
       <c r="I27" s="145"/>
     </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="141">
         <v>16</v>
       </c>
@@ -7105,7 +6878,7 @@
       <c r="H28" s="144"/>
       <c r="I28" s="145"/>
     </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="141">
         <v>17</v>
       </c>
@@ -7120,7 +6893,7 @@
       <c r="H29" s="144"/>
       <c r="I29" s="145"/>
     </row>
-    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="141">
         <v>18</v>
       </c>
@@ -7135,7 +6908,7 @@
       <c r="H30" s="144"/>
       <c r="I30" s="145"/>
     </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A31" s="141" t="s">
         <v>63</v>
       </c>
@@ -7160,7 +6933,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="11"/>
       <c r="B32" s="186"/>
       <c r="C32" s="162" t="s">
@@ -7175,7 +6948,7 @@
       <c r="H32" s="191"/>
       <c r="I32" s="190"/>
     </row>
-    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A33" s="11"/>
       <c r="B33" s="186"/>
       <c r="C33" s="186"/>
@@ -7186,7 +6959,7 @@
       <c r="H33" s="187"/>
       <c r="I33" s="188"/>
     </row>
-    <row r="34" spans="1:9" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="24.95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A34" s="181" t="s">
         <v>63</v>
       </c>
@@ -7201,7 +6974,7 @@
       <c r="H34" s="152"/>
       <c r="I34" s="153"/>
     </row>
-    <row r="35" spans="1:9" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="24.95" customHeight="1" thickTop="1">
       <c r="A35" s="183"/>
       <c r="B35" s="184">
         <v>1</v>
@@ -7218,7 +6991,7 @@
       <c r="H35" s="144"/>
       <c r="I35" s="155"/>
     </row>
-    <row r="36" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="24.95" customHeight="1">
       <c r="A36" s="183"/>
       <c r="B36" s="184">
         <v>2</v>
@@ -7235,7 +7008,7 @@
       <c r="H36" s="144"/>
       <c r="I36" s="155"/>
     </row>
-    <row r="37" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="24.95" customHeight="1">
       <c r="A37" s="183"/>
       <c r="B37" s="184">
         <v>3</v>
@@ -7250,7 +7023,7 @@
       <c r="H37" s="144"/>
       <c r="I37" s="145"/>
     </row>
-    <row r="38" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="24.95" customHeight="1">
       <c r="A38" s="183"/>
       <c r="B38" s="184">
         <v>4</v>
@@ -7265,7 +7038,7 @@
       <c r="H38" s="144"/>
       <c r="I38" s="145"/>
     </row>
-    <row r="39" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="24.95" customHeight="1">
       <c r="A39" s="183"/>
       <c r="B39" s="184">
         <v>5</v>
@@ -7280,7 +7053,7 @@
       <c r="H39" s="144"/>
       <c r="I39" s="155"/>
     </row>
-    <row r="40" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="24.95" customHeight="1">
       <c r="A40" s="183"/>
       <c r="B40" s="184">
         <v>6</v>
@@ -7295,7 +7068,7 @@
       <c r="H40" s="144"/>
       <c r="I40" s="145"/>
     </row>
-    <row r="41" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="24.95" customHeight="1">
       <c r="A41" s="183"/>
       <c r="B41" s="184">
         <v>7</v>
@@ -7310,7 +7083,7 @@
       <c r="H41" s="158"/>
       <c r="I41" s="145"/>
     </row>
-    <row r="42" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="24.95" customHeight="1">
       <c r="A42" s="183"/>
       <c r="B42" s="184">
         <v>8</v>
@@ -7325,7 +7098,7 @@
       <c r="H42" s="144"/>
       <c r="I42" s="145"/>
     </row>
-    <row r="43" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="24.95" customHeight="1">
       <c r="A43" s="183"/>
       <c r="B43" s="184">
         <v>9</v>
@@ -7340,7 +7113,7 @@
       <c r="H43" s="144"/>
       <c r="I43" s="145"/>
     </row>
-    <row r="44" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="24.95" customHeight="1">
       <c r="A44" s="183"/>
       <c r="B44" s="184">
         <v>10</v>
@@ -7353,7 +7126,7 @@
       <c r="H44" s="144"/>
       <c r="I44" s="145"/>
     </row>
-    <row r="45" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="24.95" customHeight="1">
       <c r="A45" s="183"/>
       <c r="B45" s="184">
         <v>11</v>
@@ -7366,7 +7139,7 @@
       <c r="H45" s="144"/>
       <c r="I45" s="145"/>
     </row>
-    <row r="46" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="24.95" customHeight="1" thickBot="1">
       <c r="A46" s="149"/>
       <c r="B46" s="157"/>
       <c r="C46" s="159" t="s">
@@ -7381,7 +7154,7 @@
       <c r="H46" s="150"/>
       <c r="I46" s="151"/>
     </row>
-    <row r="47" spans="1:9" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="24.95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A47" s="160"/>
       <c r="B47" s="161"/>
       <c r="C47" s="194" t="s">
@@ -7396,7 +7169,7 @@
       <c r="H47" s="163"/>
       <c r="I47" s="164"/>
     </row>
-    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A48" s="165"/>
       <c r="B48" s="165"/>
       <c r="C48" s="166"/>
@@ -7407,7 +7180,7 @@
       <c r="H48" s="167"/>
       <c r="I48" s="168"/>
     </row>
-    <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="165"/>
       <c r="B49" s="165"/>
       <c r="C49" s="166"/>
@@ -7418,7 +7191,7 @@
       <c r="H49" s="167"/>
       <c r="I49" s="167"/>
     </row>
-    <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="40"/>
       <c r="B50" s="41"/>
       <c r="C50" s="42"/>
@@ -7430,7 +7203,7 @@
       <c r="H50" s="167"/>
       <c r="I50" s="167"/>
     </row>
-    <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="45" t="s">
         <v>0</v>
       </c>
@@ -7442,7 +7215,7 @@
       <c r="H51" s="167"/>
       <c r="I51" s="167"/>
     </row>
-    <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="45" t="s">
         <v>1</v>
       </c>
@@ -7462,7 +7235,7 @@
       <c r="H52" s="167"/>
       <c r="I52" s="167"/>
     </row>
-    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="45"/>
       <c r="B53" s="228" t="s">
         <v>97</v>
@@ -7474,7 +7247,7 @@
       <c r="H53" s="167"/>
       <c r="I53" s="167"/>
     </row>
-    <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="45"/>
       <c r="B54" s="7"/>
       <c r="C54" s="6"/>
@@ -7490,7 +7263,7 @@
       <c r="H54" s="167"/>
       <c r="I54" s="167"/>
     </row>
-    <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="45"/>
       <c r="B55" s="7"/>
       <c r="C55" s="6"/>
@@ -7500,7 +7273,7 @@
       <c r="H55" s="167"/>
       <c r="I55" s="167"/>
     </row>
-    <row r="56" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A56" s="88"/>
       <c r="B56" s="89"/>
       <c r="C56" s="90"/>
@@ -7516,7 +7289,7 @@
       <c r="H56" s="167"/>
       <c r="I56" s="167"/>
     </row>
-    <row r="57" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="43"/>
       <c r="B57" s="7"/>
       <c r="C57" s="6"/>
@@ -7526,7 +7299,7 @@
       <c r="H57" s="167"/>
       <c r="I57" s="167"/>
     </row>
-    <row r="58" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="44" t="s">
         <v>6</v>
       </c>
@@ -7546,7 +7319,7 @@
       <c r="H58" s="167"/>
       <c r="I58" s="167"/>
     </row>
-    <row r="59" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="56"/>
       <c r="B59" s="54" t="s">
         <v>10</v>
@@ -7558,7 +7331,7 @@
       <c r="H59" s="167"/>
       <c r="I59" s="167"/>
     </row>
-    <row r="60" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="56"/>
       <c r="B60" s="54" t="s">
         <v>8</v>
@@ -7570,7 +7343,7 @@
       <c r="H60" s="167"/>
       <c r="I60" s="167"/>
     </row>
-    <row r="61" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="56"/>
       <c r="B61" s="54" t="s">
         <v>39</v>
@@ -7582,7 +7355,7 @@
       <c r="H61" s="167"/>
       <c r="I61" s="167"/>
     </row>
-    <row r="62" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A62" s="49"/>
       <c r="B62" s="51" t="s">
         <v>53</v>
@@ -7594,7 +7367,7 @@
       <c r="H62" s="167"/>
       <c r="I62" s="167"/>
     </row>
-    <row r="63" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A63" s="48"/>
       <c r="B63" s="50" t="s">
         <v>21</v>
@@ -7612,7 +7385,7 @@
       <c r="H63" s="167"/>
       <c r="I63" s="167"/>
     </row>
-    <row r="64" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -7622,7 +7395,7 @@
       <c r="H64" s="167"/>
       <c r="I64" s="167"/>
     </row>
-    <row r="65" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="165"/>
       <c r="B65" s="185" t="s">
         <v>11</v>
@@ -7630,14 +7403,14 @@
       <c r="C65" s="9"/>
       <c r="D65" s="167"/>
       <c r="E65" s="288" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F65" s="288"/>
       <c r="G65" s="288"/>
       <c r="H65" s="288"/>
       <c r="I65" s="288"/>
     </row>
-    <row r="66" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="165"/>
       <c r="B66" s="185" t="s">
         <v>13</v>
@@ -7650,7 +7423,7 @@
       <c r="H66" s="167"/>
       <c r="I66" s="167"/>
     </row>
-    <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" s="165"/>
       <c r="B67" s="8" t="s">
         <v>12</v>
@@ -7658,14 +7431,14 @@
       <c r="C67" s="8"/>
       <c r="D67" s="169"/>
       <c r="E67" s="289" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F67" s="289"/>
       <c r="G67" s="289"/>
       <c r="H67" s="289"/>
       <c r="I67" s="289"/>
     </row>
-    <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" s="165"/>
       <c r="B68" s="14" t="s">
         <v>16</v>
@@ -7680,7 +7453,7 @@
       <c r="H68" s="289"/>
       <c r="I68" s="289"/>
     </row>
-    <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" s="165"/>
       <c r="D69" s="169"/>
       <c r="E69" s="170"/>
@@ -7689,7 +7462,7 @@
       <c r="H69" s="170"/>
       <c r="I69" s="170"/>
     </row>
-    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" s="165"/>
       <c r="B70" s="6"/>
       <c r="C70" s="66"/>
@@ -7700,7 +7473,7 @@
       <c r="H70" s="170"/>
       <c r="I70" s="170"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9">
       <c r="A71" s="165"/>
       <c r="B71" s="233"/>
       <c r="C71" s="233"/>
@@ -7711,7 +7484,7 @@
       <c r="H71" s="171"/>
       <c r="I71" s="104"/>
     </row>
-    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="18">
       <c r="A72" s="172" t="s">
         <v>63</v>
       </c>
@@ -7734,7 +7507,7 @@
       </c>
       <c r="I72" s="173"/>
     </row>
-    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="18">
       <c r="A73" s="172"/>
       <c r="B73" s="232"/>
       <c r="C73" s="232"/>
@@ -7747,7 +7520,7 @@
       <c r="H73" s="176"/>
       <c r="I73" s="173"/>
     </row>
-    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="18">
       <c r="A74" s="172" t="s">
         <v>63</v>
       </c>
@@ -7766,7 +7539,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="18">
       <c r="A75" s="172"/>
       <c r="B75" s="233" t="s">
         <v>45</v>
@@ -7779,7 +7552,7 @@
       <c r="H75" s="176"/>
       <c r="I75" s="173"/>
     </row>
-    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="18">
       <c r="A76" s="177" t="s">
         <v>63</v>
       </c>
@@ -7798,7 +7571,7 @@
       </c>
       <c r="I76" s="178"/>
     </row>
-    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="18">
       <c r="A77" s="177"/>
       <c r="B77" s="233"/>
       <c r="C77" s="233"/>
@@ -7809,7 +7582,7 @@
       <c r="H77" s="178"/>
       <c r="I77" s="178"/>
     </row>
-    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="18">
       <c r="A78" s="177" t="s">
         <v>63</v>
       </c>
@@ -7828,7 +7601,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="18">
       <c r="A79" s="177"/>
       <c r="B79" s="232"/>
       <c r="C79" s="232"/>
@@ -7843,7 +7616,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="18">
       <c r="A80" s="177" t="s">
         <v>63</v>
       </c>
@@ -7862,7 +7635,7 @@
       </c>
       <c r="I80" s="178"/>
     </row>
-    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="18">
       <c r="A81" s="177" t="s">
         <v>63</v>
       </c>
@@ -7881,7 +7654,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="18">
       <c r="A82" s="177" t="s">
         <v>63</v>
       </c>
@@ -7900,7 +7673,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="18">
       <c r="A83" s="177"/>
       <c r="B83" s="233"/>
       <c r="C83" s="233"/>
@@ -7919,7 +7692,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="18">
       <c r="A84" s="177" t="s">
         <v>63</v>
       </c>
@@ -7938,7 +7711,7 @@
       </c>
       <c r="I84" s="178"/>
     </row>
-    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="18">
       <c r="A85" s="177"/>
       <c r="B85" s="232"/>
       <c r="C85" s="232"/>
@@ -7951,7 +7724,7 @@
       <c r="H85" s="178"/>
       <c r="I85" s="178"/>
     </row>
-    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="18">
       <c r="A86" s="177"/>
       <c r="B86" s="6"/>
       <c r="C86" s="66"/>
@@ -7962,7 +7735,7 @@
       <c r="H86" s="178"/>
       <c r="I86" s="178"/>
     </row>
-    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="18">
       <c r="A87" s="177"/>
       <c r="B87" s="233" t="s">
         <v>45</v>
@@ -7975,7 +7748,7 @@
       <c r="H87" s="178"/>
       <c r="I87" s="178"/>
     </row>
-    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="18">
       <c r="A88" s="177"/>
       <c r="B88" s="177"/>
       <c r="C88" s="178"/>
@@ -7986,7 +7759,7 @@
       <c r="H88" s="178"/>
       <c r="I88" s="178"/>
     </row>
-    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="18">
       <c r="A89" s="177"/>
       <c r="B89" s="177"/>
       <c r="C89" s="178"/>
@@ -7997,7 +7770,7 @@
       <c r="H89" s="178"/>
       <c r="I89" s="178"/>
     </row>
-    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="18">
       <c r="A90" s="178"/>
       <c r="B90" s="178"/>
       <c r="C90" s="178"/>
@@ -8008,7 +7781,7 @@
       <c r="H90" s="178"/>
       <c r="I90" s="178"/>
     </row>
-    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="18">
       <c r="A91" s="178"/>
       <c r="B91" s="178"/>
       <c r="C91" s="178"/>
@@ -8021,7 +7794,7 @@
       <c r="H91" s="178"/>
       <c r="I91" s="178"/>
     </row>
-    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="18">
       <c r="A92" s="178"/>
       <c r="B92" s="178"/>
       <c r="C92" s="178"/>
@@ -8032,7 +7805,7 @@
       <c r="H92" s="178"/>
       <c r="I92" s="178"/>
     </row>
-    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="18">
       <c r="A93" s="178"/>
       <c r="B93" s="178"/>
       <c r="C93" s="178"/>
@@ -8045,7 +7818,7 @@
       <c r="H93" s="178"/>
       <c r="I93" s="178"/>
     </row>
-    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="18">
       <c r="A94" s="178"/>
       <c r="B94" s="178"/>
       <c r="C94" s="178"/>
@@ -8056,7 +7829,7 @@
       <c r="H94" s="178"/>
       <c r="I94" s="178"/>
     </row>
-    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="18">
       <c r="A95" s="178"/>
       <c r="B95" s="178"/>
       <c r="C95" s="178"/>
@@ -8067,7 +7840,7 @@
       <c r="H95" s="178"/>
       <c r="I95" s="178"/>
     </row>
-    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="18">
       <c r="A96" s="178"/>
       <c r="B96" s="178"/>
       <c r="C96" s="178"/>
@@ -8078,7 +7851,7 @@
       <c r="H96" s="178"/>
       <c r="I96" s="178"/>
     </row>
-    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="18">
       <c r="A97" s="178"/>
       <c r="B97" s="178"/>
       <c r="C97" s="178"/>
@@ -8089,7 +7862,7 @@
       <c r="H97" s="178"/>
       <c r="I97" s="178"/>
     </row>
-    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="18">
       <c r="A98" s="178"/>
       <c r="B98" s="178"/>
       <c r="C98" s="178"/>
@@ -8100,7 +7873,7 @@
       <c r="H98" s="178"/>
       <c r="I98" s="178"/>
     </row>
-    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="18">
       <c r="A99" s="178"/>
       <c r="B99" s="178"/>
       <c r="C99" s="178"/>
@@ -8111,7 +7884,7 @@
       <c r="H99" s="178"/>
       <c r="I99" s="178"/>
     </row>
-    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="18">
       <c r="A100" s="178"/>
       <c r="B100" s="178"/>
       <c r="C100" s="178"/>
@@ -8124,7 +7897,7 @@
       <c r="H100" s="178"/>
       <c r="I100" s="178"/>
     </row>
-    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="18">
       <c r="A101" s="178"/>
       <c r="B101" s="178"/>
       <c r="C101" s="178"/>
@@ -8135,7 +7908,7 @@
       <c r="H101" s="178"/>
       <c r="I101" s="178"/>
     </row>
-    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="18">
       <c r="A102" s="178"/>
       <c r="B102" s="178"/>
       <c r="C102" s="178"/>
@@ -8146,7 +7919,7 @@
       <c r="H102" s="178"/>
       <c r="I102" s="178"/>
     </row>
-    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="18">
       <c r="A103" s="178"/>
       <c r="B103" s="178"/>
       <c r="C103" s="178"/>

</xml_diff>